<commit_message>
Finalização do trabalho de detalhamento de QT x VL (internação e ambulatório)
</commit_message>
<xml_diff>
--- a/Analise_QT_VL_Beneficiário/VV_extract_sqlbi_m18.xlsx
+++ b/Analise_QT_VL_Beneficiário/VV_extract_sqlbi_m18.xlsx
@@ -2747,6 +2747,66 @@
         <v>0.27851778210993144</v>
       </c>
     </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2017</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>201708</t>
+        </is>
+      </c>
+      <c r="C45" s="1" t="n">
+        <v>1.019738538E7</v>
+      </c>
+      <c r="D45" s="1" t="n">
+        <v>79.02</v>
+      </c>
+      <c r="E45" s="1" t="n">
+        <v>271.15</v>
+      </c>
+      <c r="F45" s="1" t="n">
+        <v>139.21</v>
+      </c>
+      <c r="G45" s="1" t="n">
+        <v>48.3</v>
+      </c>
+      <c r="H45" s="1" t="n">
+        <v>514417.0</v>
+      </c>
+      <c r="I45" s="1" t="n">
+        <v>3.99</v>
+      </c>
+      <c r="J45" s="1" t="n">
+        <v>13.68</v>
+      </c>
+      <c r="K45" s="1" t="n">
+        <v>7.02</v>
+      </c>
+      <c r="L45" s="1" t="n">
+        <v>2.44</v>
+      </c>
+      <c r="M45" s="1" t="n">
+        <v>19.823188930381384</v>
+      </c>
+      <c r="N45" s="1" t="n">
+        <v>129040.0</v>
+      </c>
+      <c r="O45" s="1" t="n">
+        <v>37608.0</v>
+      </c>
+      <c r="P45" s="1" t="n">
+        <v>73252.0</v>
+      </c>
+      <c r="Q45" s="1" t="n">
+        <v>211147.0</v>
+      </c>
+      <c r="R45" s="1" t="n">
+        <v>0.29144451332920024</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -2785,17 +2845,21 @@
         (select  to_char(pcm.mes_ano_ref,'RRRRMM') anomes,
                 sum(qtd_ativos) BT
         from    ts.posicao_cadastro_mes pcm           
-        where   pcm.mes_ano_ref between to_date ('01/01/2014','dd/mm/yyyy') and to_date ('01/07/2017','dd/mm/yyyy')
+        where   pcm.mes_ano_ref between to_date ('01/01/2014','dd/mm/yyyy') and to_date ('01/08/2017','dd/mm/yyyy')
+        --and     pcm.COD_FAIXA_ETARIA = 10
         and     pcm.COD_FAIXA_ETARIA = 1
+        --and     pcm.COD_FAIXA_ETARIA not in (1, 10)        
         group by   
                 to_char(pcm.mes_ano_ref,'RRRRMM')
         order by 1) tbt,
-        (select  b.COD_TS,
+        /**/(select  b.COD_TS,
                 b.NOME_ASSOCIADO,
                 b.DATA_NASCIMENTO,
                 2017-to_number(to_char(b.DATA_NASCIMENTO,'RRRR')) idade
         from    ts.dim_beneficiario b
+        --where   2017-to_number(to_char(b.DATA_NASCIMENTO,'RRRR')) &gt; 58) bnf
         where   2017-to_number(to_char(b.DATA_NASCIMENTO,'RRRR')) &lt; 19) bnf
+        --where   2017-to_number(to_char(b.DATA_NASCIMENTO,'RRRR')) between 19 and 58) bnf        
 where   substr(fc.ID_TEMPO_MES_ANO_REF,1,6) = tbt.anomes
 and     fc.COD_TS = bnf.COD_TS
 --and     substr(fc.ID_TEMPO_MES_ANO_REF,1,6) in ('201605')--, '201606', '201705', '201706')

</xml_diff>